<commit_message>
Completed more testing on the gui.
</commit_message>
<xml_diff>
--- a/proj_extras/Manual Testing.xlsx
+++ b/proj_extras/Manual Testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucliveac-my.sharepoint.com/personal/cgo80_uclive_ac_nz/Documents/SENG201/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\SENG201\team-56\proj_extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{983B4C60-E532-4CB0-8710-B691D9BBBF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8A68EB3-188A-448A-B14B-3FBA5582F1E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC9295-2A08-473E-8ACF-E4484556D900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual testing records" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Feature</t>
   </si>
@@ -186,6 +186,40 @@
   </si>
   <si>
     <t>The button initially update with Towers name but doesn't update when another one of the selected Tower buttons is pressed</t>
+  </si>
+  <si>
+    <t>Brought label</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click on shop tab
+4. Click on one of the items in the shop
+5. Click the buy button</t>
+  </si>
+  <si>
+    <t>Label pops up for 3 seconds then disapears to give feedback to the player</t>
+  </si>
+  <si>
+    <t>The label pops up then disapears after 3 seconds</t>
+  </si>
+  <si>
+    <t>Updating money after tower is brought</t>
+  </si>
+  <si>
+    <t>Updating money</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click on shop tab
+4. Click on one of the items in the shop
+5. Click the buy button
+6. Click on game tab
+7. Check if money value has been updated</t>
+  </si>
+  <si>
+    <t>The new money value is displayed when the item is brought</t>
   </si>
 </sst>
 </file>
@@ -313,10 +347,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,6 +991,61 @@
         <v>45434</v>
       </c>
     </row>
+    <row r="14" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="5">
+        <v>45435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="5">
+        <v>45435</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="5">
+        <v>45435</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete more testing for gui
</commit_message>
<xml_diff>
--- a/proj_extras/Manual Testing.xlsx
+++ b/proj_extras/Manual Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\SENG201\team-56\proj_extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC9295-2A08-473E-8ACF-E4484556D900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37500782-0700-4966-A6A8-AE38CF834D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual testing records" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>Feature</t>
   </si>
@@ -93,10 +93,6 @@
     <t>1. Run the application
 2. Click one of the 9 "Pick Starting Towers:" Buttons
 3. Click one of the 3 "Selected Towers" buttons</t>
-  </si>
-  <si>
-    <t>Update the button text with the resource type
- of the tower</t>
   </si>
   <si>
     <t>selected Towers</t>
@@ -220,6 +216,100 @@
   </si>
   <si>
     <t>The new money value is displayed when the item is brought</t>
+  </si>
+  <si>
+    <t>Swaping towers</t>
+  </si>
+  <si>
+    <t>Swaping towers from reserve to field</t>
+  </si>
+  <si>
+    <t>The tower is swaped to the field</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Select tower from the reserve towers
+4. Click field button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update the button text with the resource type
+ of the tower </t>
+  </si>
+  <si>
+    <t>Setting difficulty</t>
+  </si>
+  <si>
+    <t>The round difficulty is update for the next round</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click Set round difficulty
+4. Select one of the Options
+5. Click accept</t>
+  </si>
+  <si>
+    <t>The round difficulty is updated for the next 
+round</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>Error message when there is no towers on the field</t>
+  </si>
+  <si>
+    <t>1. Run the application 
+2. Click Play
+3. Click Play</t>
+  </si>
+  <si>
+    <t>An error message pops up alerting the player</t>
+  </si>
+  <si>
+    <t>The colour of the text should be red</t>
+  </si>
+  <si>
+    <t>The error message text is the colour red</t>
+  </si>
+  <si>
+    <t>Adding upgrade to tower</t>
+  </si>
+  <si>
+    <t>Apply the upgrade to the tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Run the application
+2. Click Play
+3. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After each round money should be added </t>
+  </si>
+  <si>
+    <t>1. Run the application 
+2. Click Play
+3. Click Set round difficulty
+4. Click one of the difficulty options
+5. Click accept</t>
+  </si>
+  <si>
+    <t>The money is updated after the round is over</t>
+  </si>
+  <si>
+    <t>Selecred tower colour</t>
+  </si>
+  <si>
+    <t>Update the colour of the tower when selected</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Select tower from the reserve towers</t>
+  </si>
+  <si>
+    <t>The tower colour is updated with the colour green to signify that the tower is selected</t>
   </si>
 </sst>
 </file>
@@ -318,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -332,6 +422,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,11 +812,51 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45436</v>
+      </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="5">
+        <v>45436</v>
+      </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -762,7 +893,7 @@
     </row>
     <row r="5" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -771,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -803,16 +934,16 @@
     </row>
     <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
@@ -826,16 +957,16 @@
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>9</v>
@@ -849,16 +980,16 @@
     </row>
     <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>9</v>
@@ -872,16 +1003,16 @@
     </row>
     <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>9</v>
@@ -895,13 +1026,13 @@
     </row>
     <row r="10" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -909,13 +1040,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>8</v>
@@ -938,16 +1069,16 @@
     </row>
     <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>9</v>
@@ -961,16 +1092,16 @@
     </row>
     <row r="13" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>8</v>
@@ -993,16 +1124,16 @@
     </row>
     <row r="14" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
@@ -1016,16 +1147,16 @@
     </row>
     <row r="15" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>8</v>
@@ -1044,6 +1175,103 @@
       </c>
       <c r="K15" s="5">
         <v>45435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="5">
+        <v>45436</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="5">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="5">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="5">
+        <v>45436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added report to proj_extras and complete more testing for gui in Manual Testing.xlsx
</commit_message>
<xml_diff>
--- a/proj_extras/Manual Testing.xlsx
+++ b/proj_extras/Manual Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\SENG201\team-56\proj_extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37500782-0700-4966-A6A8-AE38CF834D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54964E50-081F-45D8-8A61-69ADF3FA2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
   <si>
     <t>Feature</t>
   </si>
@@ -280,11 +280,6 @@
     <t>Apply the upgrade to the tower</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Run the application
-2. Click Play
-3. </t>
-  </si>
-  <si>
     <t xml:space="preserve">After each round money should be added </t>
   </si>
   <si>
@@ -310,6 +305,153 @@
   </si>
   <si>
     <t>The tower colour is updated with the colour green to signify that the tower is selected</t>
+  </si>
+  <si>
+    <t>Switching the style of the button when it's removed from reserve to field</t>
+  </si>
+  <si>
+    <t>Buying item after playing a round</t>
+  </si>
+  <si>
+    <t>A tower shouldn't be duplicated when you buy an item from the shop</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Add towers to the field
+4. Click Set round difficulty
+5. Click one of the difficulty options
+6. Click Play
+7. Click Ok
+8. Click Shop tab
+9. Select one of the items from the shop
+10. Click Buy</t>
+  </si>
+  <si>
+    <t>The item is added to your inventory or reserve towers and no duplicate tower is added to the reserve towers</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click Shop tab
+4. Select an upgrade
+5. Click buy
+6. Click on upgrade in inventory
+7. Click on tower</t>
+  </si>
+  <si>
+    <t>The upgrade has been applied to the tower</t>
+  </si>
+  <si>
+    <t>Sell item</t>
+  </si>
+  <si>
+    <t>Selling an item to the shop</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click on shop tab
+4. Click on tower in reserve tower
+5. Click on sell button</t>
+  </si>
+  <si>
+    <t>The tower is removed from the players inventory and money is updated</t>
+  </si>
+  <si>
+    <t>No difficulty selected</t>
+  </si>
+  <si>
+    <t>When the player hasn't selected a difficulty</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Select tower from reserve towers
+4. add tower to field towers
+5. Click Play</t>
+  </si>
+  <si>
+    <t>An error message pops up for 3 seconds telling that you need to select a difficulty</t>
+  </si>
+  <si>
+    <t>Buying towers</t>
+  </si>
+  <si>
+    <t>Buying towers that you sold to the shop</t>
+  </si>
+  <si>
+    <t>The tower is added back to your inventory and your money is taken</t>
+  </si>
+  <si>
+    <t>Round status</t>
+  </si>
+  <si>
+    <t>Round status labels updating distance and amount full for multiple rounds</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click on shop tab
+4. Click on tower in reserve towers
+5. Click on sell button
+6. select tower you sold to the shop
+7. Click buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Run the application
+2. Click Play
+3. Click on tower in reserve towers
+4. Click on button in field
+5. Click Set round difficulty
+6. Select one of the Options
+7. Click accept
+8. Click Play
+9. Repeat 3-8 </t>
+  </si>
+  <si>
+    <t>The round status labels are updating distance and amount full and clearing after each new round</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Click on tower in reserve tower
+4. Click on button in the field</t>
+  </si>
+  <si>
+    <t>The tower should be swapped/moved and the style of the button should be moved as well</t>
+  </si>
+  <si>
+    <t>Applying upgrades</t>
+  </si>
+  <si>
+    <t>Applying rarity upgrade to broken tower</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Play a round
+4. Buy rarity upgrade from shop
+5. apply rarity upgrade to broken tower</t>
+  </si>
+  <si>
+    <t>The upgrade shouldn't be applied to the broken tower</t>
+  </si>
+  <si>
+    <t>Inventory applying upgrades</t>
+  </si>
+  <si>
+    <t>Applying upgrades from your Inventory to a tower</t>
+  </si>
+  <si>
+    <t>1. Run the application
+2. Click Play
+3. Buy 2 upgrades from the shop
+4. Click on the upgrade
+5. Click on the tower twice</t>
+  </si>
+  <si>
+    <t>Both upgrades shouldn't be added only one you would have to select the next upgrade in inventory then select tower to add the second upgrade</t>
   </si>
 </sst>
 </file>
@@ -408,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -422,7 +564,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +968,7 @@
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="5">
@@ -1193,11 +1334,14 @@
       <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
       <c r="H16" s="5">
         <v>45436</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1213,17 +1357,23 @@
       <c r="F17" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
       <c r="H17" s="5">
         <v>45436</v>
       </c>
       <c r="I17" t="s">
         <v>9</v>
       </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
       <c r="K17" s="5">
         <v>45436</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1231,47 +1381,339 @@
         <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="5">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
       <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
       <c r="H19" s="5">
         <v>45436</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="5">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="F20" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
       </c>
       <c r="H20" s="5">
         <v>45436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="5">
+        <v>45437</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="5">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="5">
+        <v>45436</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="5">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="5">
+        <v>45437</v>
+      </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="5">
+        <v>45437</v>
+      </c>
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="5">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="5">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="5">
+        <v>45437</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="5">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="5">
+        <v>45437</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="5">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="5">
+        <v>45437</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="5">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="5">
+        <v>45437</v>
+      </c>
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="5">
+        <v>45437</v>
+      </c>
+      <c r="L28" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" s="5">
+        <v>45437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>